<commit_message>
Adding more noise results
</commit_message>
<xml_diff>
--- a/Research/Results.xlsx
+++ b/Research/Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Faults </t>
   </si>
@@ -47,6 +47,21 @@
   </si>
   <si>
     <t xml:space="preserve">Blue </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partial Occlusion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaussian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S&amp;P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poisson</t>
   </si>
 </sst>
 </file>
@@ -144,22 +159,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="29.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -179,7 +192,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
@@ -198,12 +211,8 @@
       <c r="F2" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="G2" s="0" t="e">
-        <f aca="false">D1+E1-F1</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
         <v>7</v>
       </c>
@@ -219,12 +228,8 @@
       <c r="F3" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="G3" s="0" t="n">
-        <f aca="false">D2+E2-F2</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
         <v>8</v>
       </c>
@@ -240,25 +245,82 @@
       <c r="F4" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="G4" s="0" t="n">
-        <f aca="false">D3+E3-F3</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G5" s="0" t="n">
-        <f aca="false">D4+E4-F4</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>433</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>